<commit_message>
Aktualizovane TODO s listy pro každého, nový dokument Napady na napady.
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Obecne" sheetId="1" r:id="rId1"/>
+    <sheet name="Sebastian" sheetId="2" r:id="rId2"/>
+    <sheet name="Dominik" sheetId="3" r:id="rId3"/>
+    <sheet name="prof. Marsalek" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,22 +27,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>TODO:</t>
+    <t>zkusit painlessMesh s ESP32</t>
   </si>
   <si>
-    <t>Sebastian:</t>
+    <t>Úkol</t>
   </si>
   <si>
-    <t>Zkusit painlessMesh na ESP32</t>
+    <t>splnit do</t>
+  </si>
+  <si>
+    <t>splněno</t>
+  </si>
+  <si>
+    <t>Obecné nápady</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,16 +65,46 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -73,13 +112,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -360,31 +535,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>2</v>
+    <row r="2" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="17">
+        <v>44370</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>